<commit_message>
return json by using excel
</commit_message>
<xml_diff>
--- a/MBG_products.xlsx
+++ b/MBG_products.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25329"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatrajesh/Desktop/MBG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{62AAD80F-0EF8-F84A-971F-47A5DF1E5846}" xr6:coauthVersionLast="48" xr6:coauthVersionMax="48" xr10:uidLastSave="{DBC3F799-D39F-4F18-9E68-7A83B77DF05C}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{62AAD80F-0EF8-F84A-971F-47A5DF1E5846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{0840B43B-E301-480D-B00B-795D0AB401D1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{21B20AA2-56D6-9443-8602-EEA0E832E8FD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="149">
   <si>
     <t>ProductName</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Addl_desc_product</t>
-  </si>
-  <si>
-    <t>Short Description</t>
   </si>
   <si>
     <t>prod_req_doc</t>
@@ -612,7 +609,7 @@
 &lt;/div&gt;</t>
   </si>
   <si>
-    <t>Advisory Services</t>
+    <t>Taxation Advisory Services</t>
   </si>
   <si>
     <t>&lt;div class="elementor-widget-wrap elementor-element-populated"&gt;
@@ -1198,6 +1195,9 @@
       </rPr>
       <t>&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>Legal Advisory Services</t>
   </si>
   <si>
     <t>Income tax refund</t>
@@ -5686,13 +5686,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>301625</xdr:rowOff>
@@ -6032,33 +6032,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79FFA0FD-E619-7A4D-B25A-3B4DC160B22D}">
-  <dimension ref="A1:AE144"/>
+  <dimension ref="A1:AD144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="49.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="80.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.5" customWidth="1"/>
-    <col min="28" max="28" width="19.25" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.75" customWidth="1"/>
+    <col min="6" max="6" width="32.5" customWidth="1"/>
+    <col min="7" max="7" width="22.125" customWidth="1"/>
+    <col min="8" max="8" width="6.75" customWidth="1"/>
+    <col min="9" max="9" width="3" customWidth="1"/>
+    <col min="10" max="10" width="3.125" customWidth="1"/>
+    <col min="11" max="11" width="3.25" customWidth="1"/>
+    <col min="13" max="13" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:30" ht="15.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6149,18 +6151,18 @@
       <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+    </row>
+    <row r="2" spans="1:30" ht="36" customHeight="1">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" ht="409.6">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -6169,74 +6171,73 @@
       <c r="F2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>36</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2">
+        <v>4000</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
         <v>37</v>
-      </c>
-      <c r="I2">
-        <v>4000</v>
-      </c>
-      <c r="J2">
-        <v>5</v>
       </c>
       <c r="K2" t="s">
         <v>38</v>
       </c>
-      <c r="L2" t="s">
+    </row>
+    <row r="3" spans="1:30" ht="78" customHeight="1">
+      <c r="A3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" ht="409.6">
-      <c r="A3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s">
         <v>36</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <v>4000</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
         <v>37</v>
-      </c>
-      <c r="I3">
-        <v>4000</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
       </c>
       <c r="K3" t="s">
         <v>38</v>
       </c>
-      <c r="L3" t="s">
-        <v>39</v>
-      </c>
+      <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:31" ht="409.6">
+    </row>
+    <row r="4" spans="1:30" ht="40.5" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>43</v>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>34</v>
@@ -6244,38 +6245,38 @@
       <c r="F4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
         <v>36</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4">
+        <v>4000</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
         <v>37</v>
-      </c>
-      <c r="I4">
-        <v>4000</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
       </c>
       <c r="K4" t="s">
         <v>38</v>
       </c>
-      <c r="L4" t="s">
-        <v>39</v>
-      </c>
+      <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:31" ht="409.6">
+    </row>
+    <row r="5" spans="1:30" ht="409.6">
       <c r="A5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>45</v>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>34</v>
@@ -6283,38 +6284,38 @@
       <c r="F5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" t="s">
         <v>36</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5">
+        <v>4000</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
         <v>37</v>
-      </c>
-      <c r="I5">
-        <v>4000</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
       </c>
       <c r="K5" t="s">
         <v>38</v>
       </c>
-      <c r="L5" t="s">
-        <v>39</v>
-      </c>
+      <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:31" ht="409.6">
+    </row>
+    <row r="6" spans="1:30" ht="409.6">
       <c r="A6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>47</v>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>34</v>
@@ -6322,34 +6323,34 @@
       <c r="F6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" t="s">
         <v>36</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6">
+        <v>4000</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
         <v>37</v>
-      </c>
-      <c r="I6">
-        <v>4000</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
       </c>
       <c r="K6" t="s">
         <v>38</v>
       </c>
-      <c r="L6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" ht="330">
+    </row>
+    <row r="7" spans="1:30" ht="409.6">
       <c r="A7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>49</v>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>34</v>
@@ -6357,34 +6358,34 @@
       <c r="F7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" t="s">
         <v>36</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7">
+        <v>4000</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
         <v>37</v>
       </c>
-      <c r="I7">
-        <v>4000</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
       <c r="K7" t="s">
-        <v>38</v>
-      </c>
-      <c r="L7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="409.6">
+      <c r="A8" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" ht="409.6">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>52</v>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>34</v>
@@ -6392,34 +6393,34 @@
       <c r="F8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" t="s">
         <v>36</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8">
+        <v>4000</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8" t="s">
         <v>37</v>
-      </c>
-      <c r="I8">
-        <v>4000</v>
-      </c>
-      <c r="J8">
-        <v>5</v>
       </c>
       <c r="K8" t="s">
         <v>38</v>
       </c>
-      <c r="L8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" ht="409.6">
+    </row>
+    <row r="9" spans="1:30" ht="409.6">
       <c r="A9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>54</v>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>34</v>
@@ -6427,34 +6428,34 @@
       <c r="F9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" t="s">
         <v>36</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9">
+        <v>4000</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
         <v>37</v>
-      </c>
-      <c r="I9">
-        <v>4000</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
       </c>
       <c r="K9" t="s">
         <v>38</v>
       </c>
-      <c r="L9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" ht="15.75">
+    </row>
+    <row r="10" spans="1:30" ht="15.75">
       <c r="A10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>56</v>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>34</v>
@@ -6462,38 +6463,38 @@
       <c r="F10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>57</v>
+      <c r="G10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10">
+        <v>4000</v>
       </c>
       <c r="I10">
-        <v>4000</v>
-      </c>
-      <c r="J10">
         <v>5</v>
+      </c>
+      <c r="J10" t="s">
+        <v>37</v>
       </c>
       <c r="K10" t="s">
         <v>38</v>
       </c>
-      <c r="L10" t="s">
-        <v>39</v>
-      </c>
+      <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="1:31" ht="15.75">
+    </row>
+    <row r="11" spans="1:30" ht="15.75">
       <c r="A11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>59</v>
+      <c r="D11" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>34</v>
@@ -6501,34 +6502,34 @@
       <c r="F11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>57</v>
+      <c r="G11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11">
+        <v>4000</v>
       </c>
       <c r="I11">
-        <v>4000</v>
-      </c>
-      <c r="J11">
         <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>37</v>
       </c>
       <c r="K11" t="s">
         <v>38</v>
       </c>
-      <c r="L11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" ht="409.6">
+    </row>
+    <row r="12" spans="1:30" ht="409.6">
       <c r="A12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>61</v>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>34</v>
@@ -6536,38 +6537,38 @@
       <c r="F12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>57</v>
+      <c r="G12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12">
+        <v>4000</v>
       </c>
       <c r="I12">
-        <v>4000</v>
-      </c>
-      <c r="J12">
         <v>5</v>
+      </c>
+      <c r="J12" t="s">
+        <v>37</v>
       </c>
       <c r="K12" t="s">
         <v>38</v>
       </c>
-      <c r="L12" t="s">
-        <v>39</v>
-      </c>
+      <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="1:31" ht="15.75">
+    </row>
+    <row r="13" spans="1:30" ht="15.75">
       <c r="A13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>63</v>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>34</v>
@@ -6575,34 +6576,34 @@
       <c r="F13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>57</v>
+      <c r="G13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13">
+        <v>4000</v>
       </c>
       <c r="I13">
-        <v>4000</v>
-      </c>
-      <c r="J13">
         <v>5</v>
+      </c>
+      <c r="J13" t="s">
+        <v>37</v>
       </c>
       <c r="K13" t="s">
         <v>38</v>
       </c>
-      <c r="L13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" ht="15.75">
+    </row>
+    <row r="14" spans="1:30" ht="15.75">
       <c r="A14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>65</v>
+      <c r="D14" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>34</v>
@@ -6610,38 +6611,38 @@
       <c r="F14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>57</v>
+      <c r="G14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14">
+        <v>4000</v>
       </c>
       <c r="I14">
-        <v>4000</v>
-      </c>
-      <c r="J14">
         <v>5</v>
+      </c>
+      <c r="J14" t="s">
+        <v>37</v>
       </c>
       <c r="K14" t="s">
         <v>38</v>
       </c>
-      <c r="L14" t="s">
-        <v>39</v>
-      </c>
+      <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-    </row>
-    <row r="15" spans="1:31" ht="15.75">
+    </row>
+    <row r="15" spans="1:30" ht="15.75">
       <c r="A15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>67</v>
+      <c r="D15" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>34</v>
@@ -6649,34 +6650,34 @@
       <c r="F15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>57</v>
+      <c r="G15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15">
+        <v>4000</v>
       </c>
       <c r="I15">
-        <v>4000</v>
-      </c>
-      <c r="J15">
         <v>5</v>
+      </c>
+      <c r="J15" t="s">
+        <v>37</v>
       </c>
       <c r="K15" t="s">
         <v>38</v>
       </c>
-      <c r="L15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" ht="330">
+    </row>
+    <row r="16" spans="1:30" ht="409.6">
       <c r="A16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>49</v>
+      <c r="D16" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>34</v>
@@ -6684,131 +6685,128 @@
       <c r="F16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>57</v>
+      <c r="G16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16">
+        <v>4000</v>
       </c>
       <c r="I16">
-        <v>4000</v>
-      </c>
-      <c r="J16">
         <v>5</v>
       </c>
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
       <c r="K16" t="s">
-        <v>38</v>
-      </c>
-      <c r="L16" t="s">
-        <v>50</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" ht="409.6">
+    </row>
+    <row r="17" spans="1:11" ht="409.6">
       <c r="A17" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>69</v>
       </c>
+      <c r="D17" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" t="s">
         <v>36</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17">
+        <v>4000</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
         <v>37</v>
-      </c>
-      <c r="I17">
-        <v>4000</v>
-      </c>
-      <c r="J17">
-        <v>5</v>
       </c>
       <c r="K17" t="s">
         <v>38</v>
       </c>
-      <c r="L17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.75">
+    </row>
+    <row r="18" spans="1:11" ht="15.75">
       <c r="C18" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:11" ht="15.75">
       <c r="C19" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15.75">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75">
       <c r="C20" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75"/>
-    <row r="22" spans="1:12" ht="15.75">
+    <row r="21" spans="1:11" ht="15.75"/>
+    <row r="22" spans="1:11" ht="15.75">
       <c r="C22" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75">
+    <row r="23" spans="1:11" ht="15.75">
       <c r="C23" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.75">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75">
       <c r="C24" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15.75">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75">
       <c r="C25" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75">
+    <row r="26" spans="1:11" ht="15.75">
       <c r="C26" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75">
+    <row r="27" spans="1:11" ht="15.75">
       <c r="C27" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="15.75">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75">
       <c r="C28" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75">
+    <row r="29" spans="1:11" ht="15.75">
       <c r="C29" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75">
+    <row r="30" spans="1:11" ht="15.75">
       <c r="C30" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75">
+    <row r="31" spans="1:11" ht="15.75">
       <c r="C31" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75">
+    <row r="32" spans="1:11" ht="15.75">
       <c r="C32" s="6" t="s">
         <v>79</v>
       </c>
@@ -6855,12 +6853,12 @@
     </row>
     <row r="41" spans="3:3" ht="15.75">
       <c r="C41" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="3:3" ht="15.75">
       <c r="C42" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="3:3" ht="15.75">
@@ -6875,7 +6873,7 @@
     </row>
     <row r="45" spans="3:3" ht="15.75">
       <c r="C45" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="3:3" ht="15.75">
@@ -6885,12 +6883,12 @@
     </row>
     <row r="47" spans="3:3" ht="15.75">
       <c r="C47" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="3:3" ht="15.75">
       <c r="C48" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="3:3" ht="15.75">
@@ -6905,7 +6903,7 @@
     </row>
     <row r="51" spans="3:3" ht="15.75">
       <c r="C51" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="3:3" ht="15.75">
@@ -6930,12 +6928,12 @@
     </row>
     <row r="56" spans="3:3" ht="15.75">
       <c r="C56" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="3:3" ht="15.75">
       <c r="C57" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="3:3" ht="15.75">
@@ -6950,7 +6948,7 @@
     </row>
     <row r="60" spans="3:3" ht="15.75">
       <c r="C60" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="3:3" ht="15.75">
@@ -6960,12 +6958,12 @@
     </row>
     <row r="62" spans="3:3" ht="15.75">
       <c r="C62" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="3:3" ht="15.75">
       <c r="C63" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="3:3" ht="15.75">
@@ -6980,7 +6978,7 @@
     </row>
     <row r="66" spans="3:3" ht="15.75">
       <c r="C66" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="3:3" ht="15.75">
@@ -7000,12 +6998,12 @@
     </row>
     <row r="70" spans="3:3" ht="15.75">
       <c r="C70" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="3:3" ht="15.75">
       <c r="C71" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="3:3" ht="15.75">
@@ -7020,7 +7018,7 @@
     </row>
     <row r="74" spans="3:3" ht="15.75">
       <c r="C74" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="3:3" ht="15.75">
@@ -7030,12 +7028,12 @@
     </row>
     <row r="76" spans="3:3" ht="15.75">
       <c r="C76" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="3:3" ht="15.75">
       <c r="C77" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="3:3" ht="15.75">
@@ -7050,7 +7048,7 @@
     </row>
     <row r="80" spans="3:3" ht="15.75">
       <c r="C80" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="3:3" ht="15.75">
@@ -7095,12 +7093,12 @@
     </row>
     <row r="89" spans="3:3" ht="15.75">
       <c r="C89" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="90" spans="3:3" ht="15.75">
       <c r="C90" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="91" spans="3:3" ht="15.75">
@@ -7115,7 +7113,7 @@
     </row>
     <row r="93" spans="3:3" ht="15.75">
       <c r="C93" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="3:3" ht="15.75">
@@ -7125,12 +7123,12 @@
     </row>
     <row r="95" spans="3:3" ht="15.75">
       <c r="C95" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="96" spans="3:3" ht="15.75">
       <c r="C96" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="97" spans="3:3" ht="15.75">
@@ -7145,7 +7143,7 @@
     </row>
     <row r="99" spans="3:3" ht="15.75">
       <c r="C99" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="100" spans="3:3" ht="15.75">
@@ -7215,12 +7213,12 @@
     </row>
     <row r="113" spans="3:3" ht="15.75">
       <c r="C113" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="114" spans="3:3" ht="15.75">
       <c r="C114" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="115" spans="3:3" ht="15.75">
@@ -7235,7 +7233,7 @@
     </row>
     <row r="117" spans="3:3" ht="15.75">
       <c r="C117" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="118" spans="3:3" ht="15.75">
@@ -7245,12 +7243,12 @@
     </row>
     <row r="119" spans="3:3" ht="15.75">
       <c r="C119" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="120" spans="3:3" ht="15.75">
       <c r="C120" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="121" spans="3:3" ht="15.75">
@@ -7265,7 +7263,7 @@
     </row>
     <row r="123" spans="3:3" ht="15.75">
       <c r="C123" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="124" spans="3:3" ht="15.75">
@@ -7285,12 +7283,12 @@
     </row>
     <row r="127" spans="3:3" ht="15.75">
       <c r="C127" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="128" spans="3:3" ht="15.75">
       <c r="C128" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="129" spans="3:3" ht="15.75">
@@ -7305,7 +7303,7 @@
     </row>
     <row r="131" spans="3:3" ht="15.75">
       <c r="C131" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="132" spans="3:3" ht="15.75">
@@ -7320,12 +7318,12 @@
     </row>
     <row r="134" spans="3:3" ht="15.75">
       <c r="C134" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="135" spans="3:3" ht="15.75">
       <c r="C135" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="136" spans="3:3" ht="15.75">
@@ -7340,7 +7338,7 @@
     </row>
     <row r="138" spans="3:3" ht="15.75">
       <c r="C138" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="139" spans="3:3" ht="15.75">
@@ -7360,17 +7358,17 @@
     </row>
     <row r="142" spans="3:3" ht="15.75">
       <c r="C142" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="143" spans="3:3" ht="15.75">
       <c r="C143" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="144" spans="3:3" ht="15.75">
       <c r="C144" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>